<commit_message>
Added delta and % increase to analysis
</commit_message>
<xml_diff>
--- a/ga_population.xlsx
+++ b/ga_population.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>US</t>
   </si>
@@ -34,7 +34,13 @@
     <t>GA</t>
   </si>
   <si>
-    <t>GA %</t>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>% Increase</t>
+  </si>
+  <si>
+    <t>GA % of USA</t>
   </si>
 </sst>
 </file>
@@ -78,12 +84,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -420,7 +429,7 @@
             <c:numRef>
               <c:f>Data!$B$2:$K$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2216331</c:v>
@@ -1442,18 +1451,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
-    <col min="5" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1494,34 +1502,34 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>2216331</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>2609121</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>2895832</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>2908506</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>3123723</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>3444578</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>3943116</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <v>4589575</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <v>5463105</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
         <v>6478216</v>
       </c>
     </row>
@@ -1529,40 +1537,40 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>76212168</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>92228496</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>106021537</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>123202624</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>132164569</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <v>151325798</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>179323175</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
         <v>203211926</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="3">
         <v>226545805</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
         <v>248709873</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:K4" si="0">B2/B3</f>
@@ -1603,6 +1611,89 @@
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>2.6047281203026469E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
+        <f>C2-B2</f>
+        <v>392790</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:K5" si="1">D2-C2</f>
+        <v>286711</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>12674</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>215217</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="1"/>
+        <v>320855</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="1"/>
+        <v>498538</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="1"/>
+        <v>646459</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="1"/>
+        <v>873530</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>1015111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <f>C2/B2-1</f>
+        <v>0.17722533321963185</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" ref="D6:J6" si="2">D2/C2-1</f>
+        <v>0.10988796610046059</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="2"/>
+        <v>4.3766351086664823E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="2"/>
+        <v>7.3995721514757085E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.10271557369203355</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.14473122687307405</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1639462293272631</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.19032916991224669</v>
+      </c>
+      <c r="K6" s="2">
+        <f>K2/J2-1</f>
+        <v>0.18581209769901919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Y axis and updated title
</commit_message>
<xml_diff>
--- a/ga_population.xlsx
+++ b/ga_population.xlsx
@@ -166,7 +166,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000"/>
-              <a:t>Georgia Population, in millions</a:t>
+              <a:t>GA</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t> and AL</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t> Population, in millions</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -217,9 +225,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.709665138011595E-2"/>
+          <c:x val="4.9001413284877858E-2"/>
           <c:y val="0.14397369769020929"/>
-          <c:w val="0.86601690173343715"/>
+          <c:w val="0.90411213982867511"/>
           <c:h val="0.79051623842027308"/>
         </c:manualLayout>
       </c:layout>
@@ -279,18 +287,14 @@
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -304,9 +308,7 @@
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -334,8 +336,8 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.4998397877178598E-2"/>
-                  <c:y val="-3.3496665733019834E-2"/>
+                  <c:x val="-6.3789564765942719E-2"/>
+                  <c:y val="-3.1479544633320228E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -533,45 +535,35 @@
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -732,8 +724,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="128561128"/>
-        <c:axId val="128567008"/>
+        <c:axId val="361138488"/>
+        <c:axId val="361140840"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -880,7 +872,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$A$4</c15:sqref>
@@ -921,7 +913,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$B$1:$K$1</c15:sqref>
@@ -966,7 +958,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$B$4:$K$4</c15:sqref>
@@ -1018,7 +1010,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$A$5</c15:sqref>
@@ -1059,7 +1051,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$B$1:$K$1</c15:sqref>
@@ -1104,7 +1096,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$B$5:$K$5</c15:sqref>
@@ -1153,7 +1145,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$A$6</c15:sqref>
@@ -1194,7 +1186,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$B$1:$K$1</c15:sqref>
@@ -1239,7 +1231,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Data!$B$6:$K$6</c15:sqref>
@@ -1286,7 +1278,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128561128"/>
+        <c:axId val="361138488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,7 +1321,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128567008"/>
+        <c:crossAx val="361140840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1337,44 +1329,17 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128567008"/>
+        <c:axId val="361140840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00,,\ &quot;M&quot;" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="128561128"/>
+        <c:crossAx val="361138488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1961,7 +1926,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added AL % of USA population
</commit_message>
<xml_diff>
--- a/ga_population.xlsx
+++ b/ga_population.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>US</t>
   </si>
@@ -45,12 +45,15 @@
   <si>
     <t>AL</t>
   </si>
+  <si>
+    <t>AL % of USA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,12 +67,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,7 +90,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -103,9 +100,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -570,9 +564,7 @@
               <c:idx val="8"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="0.00,,\ &quot;M&quot;" sourceLinked="0"/>
@@ -724,8 +716,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="361138488"/>
-        <c:axId val="361140840"/>
+        <c:axId val="340292120"/>
+        <c:axId val="340297216"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1278,7 +1270,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361138488"/>
+        <c:axId val="340292120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1313,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361140840"/>
+        <c:crossAx val="340297216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1329,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361140840"/>
+        <c:axId val="340297216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,7 +1331,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="361138488"/>
+        <c:crossAx val="340292120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1926,7 +1918,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0"/>
+    <sheetView zoomScale="70" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1937,7 +1929,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:ext cx="8657167" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2372,8 +2364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,7 +2643,49 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <f>B7/B3</f>
+        <v>2.3994816680716916E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:K8" si="3">C7/C3</f>
+        <v>2.3182563879172443E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="3"/>
+        <v>2.2148084874491113E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1478828243138716E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1435101869094735E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0232789388627576E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="3"/>
+        <v>1.8217054209529807E-2</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6948636174040296E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7188082560169234E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6246186575793877E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added AL year over year population delta
</commit_message>
<xml_diff>
--- a/ga_population.xlsx
+++ b/ga_population.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>US</t>
   </si>
@@ -491,7 +491,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$7</c:f>
+              <c:f>Data!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -667,7 +667,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$7:$K$7</c:f>
+              <c:f>Data!$B$8:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2362,10 +2362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:K8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2608,83 +2608,135 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1828697</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2138093</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2348174</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2646248</v>
-      </c>
-      <c r="F7" s="3">
-        <v>2832961</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3061743</v>
-      </c>
-      <c r="H7" s="3">
-        <v>3266740</v>
-      </c>
-      <c r="I7" s="3">
-        <v>3444165</v>
-      </c>
-      <c r="J7" s="3">
-        <v>3893888</v>
-      </c>
-      <c r="K7" s="3">
-        <v>4040587</v>
-      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1828697</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2138093</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2348174</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2646248</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2832961</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3061743</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3266740</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3444165</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3893888</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4040587</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <f>B7/B3</f>
+      <c r="B9" s="2">
+        <f>B8/B3</f>
         <v>2.3994816680716916E-2</v>
       </c>
-      <c r="C8" s="2">
-        <f t="shared" ref="C8:K8" si="3">C7/C3</f>
+      <c r="C9" s="2">
+        <f t="shared" ref="C9:K9" si="3">C8/C3</f>
         <v>2.3182563879172443E-2</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <f t="shared" si="3"/>
         <v>2.2148084874491113E-2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <f t="shared" si="3"/>
         <v>2.1478828243138716E-2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <f t="shared" si="3"/>
         <v>2.1435101869094735E-2</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <f t="shared" si="3"/>
         <v>2.0232789388627576E-2</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <f t="shared" si="3"/>
         <v>1.8217054209529807E-2</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I9" s="2">
         <f t="shared" si="3"/>
         <v>1.6948636174040296E-2</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J9" s="2">
         <f t="shared" si="3"/>
         <v>1.7188082560169234E-2</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K9" s="2">
         <f t="shared" si="3"/>
         <v>1.6246186575793877E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <f>C8-B8</f>
+        <v>309396</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ref="D10:K10" si="4">D8-C8</f>
+        <v>210081</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="4"/>
+        <v>298074</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="4"/>
+        <v>186713</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="4"/>
+        <v>228782</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="4"/>
+        <v>204997</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="4"/>
+        <v>177425</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="4"/>
+        <v>449723</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="4"/>
+        <v>146699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated chart title to include TN
</commit_message>
<xml_diff>
--- a/ga_population.xlsx
+++ b/ga_population.xlsx
@@ -166,11 +166,19 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2000" baseline="0"/>
-              <a:t> and AL</a:t>
+              <a:t>, AL</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2000"/>
-              <a:t> Population, in millions</a:t>
+              <a:t> and TN Population</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t> (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>millions)</a:t>
             </a:r>
           </a:p>
           <a:p>

</xml_diff>